<commit_message>
Adiccionar Chave do Cte para importação do XML
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\Área de Trabalho\api-SAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C48B82A-96F9-4712-9CEF-259DC3AD8F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F4226D-88C9-4A3D-9AC0-206DFC903FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{D08BD022-43C2-45AB-9AC6-0B15B278853A}"/>
   </bookViews>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>numeroAutorizacao</t>
+    <t>Ordem autorização</t>
   </si>
   <si>
-    <t>externalId</t>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CAE0D-2BC0-4C34-9C15-6DB595E2F40F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,10 +413,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>123</v>
+        <v>1037083</v>
       </c>
       <c r="B2">
-        <v>456</v>
+        <v>34130918</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1036133</v>
+      </c>
+      <c r="B3">
+        <v>34131096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>